<commit_message>
Test Cases and Execution Report folder and file Committed
</commit_message>
<xml_diff>
--- a/Test Cases and Execution Report/Test Cases and Execution Report.xlsx
+++ b/Test Cases and Execution Report/Test Cases and Execution Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azansari/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azansari/Documents/GitHub/mobile-test/Test Cases and Execution Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBCB98D-DE78-2844-B446-DCFF0D668201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2635E7-EB2B-6946-96CE-D4E56B8DD8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F616D8E3-1D36-B54C-A515-2C861EC6B1A8}"/>
   </bookViews>
@@ -16,12 +16,6 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case Execution Report" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Test Case Execution Report'!$D$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Test Case Execution Report'!$D$8:$I$8</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Test Case Execution Report'!$D$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Test Case Execution Report'!$D$8:$I$8</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
   <si>
     <t>TC - 01: To verify if user is able to search a city using the search box</t>
   </si>
@@ -209,6 +203,18 @@
   </si>
   <si>
     <t>Minor</t>
+  </si>
+  <si>
+    <t>TC - 06: To verify that when user is on the Map screen landing page, Google map is interactable</t>
+  </si>
+  <si>
+    <t>Google Map should be interactable</t>
+  </si>
+  <si>
+    <t>Verify that user is able to interact with the Google Map</t>
+  </si>
+  <si>
+    <t>Google Map is not interactable</t>
   </si>
 </sst>
 </file>
@@ -465,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -489,22 +495,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -522,6 +513,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -530,15 +548,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,10 +823,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1072,10 +1081,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -2737,10 +2746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E37929-D6B4-9047-8925-B9A643706CC6}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2753,22 +2762,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25"/>
     </row>
     <row r="2" spans="1:5" ht="21">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="1:5" ht="21">
       <c r="A3" s="1" t="s">
@@ -2857,22 +2866,22 @@
     </row>
     <row r="9" spans="1:5" ht="17" thickBot="1"/>
     <row r="10" spans="1:5" ht="21">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="1:5" ht="21">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="16"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:5" ht="21">
       <c r="A12" s="1" t="s">
@@ -2961,22 +2970,22 @@
     </row>
     <row r="18" spans="1:5" ht="17" thickBot="1"/>
     <row r="19" spans="1:5" ht="21">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="25"/>
     </row>
     <row r="20" spans="1:5" ht="21">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="16"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21" spans="1:5" ht="21">
       <c r="A21" s="1" t="s">
@@ -3033,7 +3042,7 @@
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="12" t="s">
         <v>34</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -3048,22 +3057,22 @@
     </row>
     <row r="26" spans="1:5" ht="17" thickBot="1"/>
     <row r="27" spans="1:5" ht="21">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25"/>
     </row>
     <row r="28" spans="1:5" ht="21">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29" spans="1:5" ht="21">
       <c r="A29" s="1" t="s">
@@ -3118,22 +3127,22 @@
     </row>
     <row r="33" spans="1:5" ht="17" thickBot="1"/>
     <row r="34" spans="1:5" ht="21">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
     </row>
     <row r="35" spans="1:5" ht="21">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="1:5" ht="21">
       <c r="A36" s="1" t="s">
@@ -3186,18 +3195,124 @@
         <v>10</v>
       </c>
     </row>
+    <row r="40" spans="1:5" ht="17" thickBot="1"/>
+    <row r="41" spans="1:5" ht="21">
+      <c r="A41" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+    </row>
+    <row r="42" spans="1:5" ht="21">
+      <c r="A42" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="22"/>
+    </row>
+    <row r="43" spans="1:5" ht="21">
+      <c r="A43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="44">
+      <c r="A44" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="21">
+      <c r="A45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="21">
+      <c r="A46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="45" thickBot="1">
+      <c r="A47" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A27:E27"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A34:E34"/>
     <mergeCell ref="A35:E35"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3221,89 +3336,89 @@
   <sheetData>
     <row r="5" spans="4:9" ht="17" thickBot="1"/>
     <row r="6" spans="4:9" ht="24">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="24"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
     </row>
     <row r="7" spans="4:9" ht="44">
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="18" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="4:9" ht="22" thickBot="1">
       <c r="D8" s="8">
-        <v>5</v>
-      </c>
-      <c r="E8" s="20">
+        <v>6</v>
+      </c>
+      <c r="E8" s="15">
         <v>2</v>
       </c>
-      <c r="F8" s="20">
-        <v>3</v>
-      </c>
-      <c r="G8" s="20">
+      <c r="F8" s="15">
+        <v>4</v>
+      </c>
+      <c r="G8" s="15">
+        <v>19</v>
+      </c>
+      <c r="H8" s="15">
         <v>15</v>
       </c>
-      <c r="H8" s="20">
-        <v>12</v>
-      </c>
-      <c r="I8" s="21">
-        <v>3</v>
+      <c r="I8" s="16">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="5:8" ht="17" thickBot="1"/>
     <row r="24" spans="5:8" ht="24">
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28"/>
     </row>
     <row r="25" spans="5:8" ht="44">
-      <c r="E25" s="27" t="s">
+      <c r="E25" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H25" s="18" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="5:8" ht="22" thickBot="1">
       <c r="E26" s="8">
+        <v>4</v>
+      </c>
+      <c r="F26" s="13">
         <v>3</v>
       </c>
-      <c r="F26" s="18">
-        <v>2</v>
-      </c>
-      <c r="G26" s="18">
+      <c r="G26" s="13">
         <v>1</v>
       </c>
-      <c r="H26" s="19">
+      <c r="H26" s="14">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final Commit Test Assignment
Deliverables

1. Manual test cases - 8 Test cases Created (Maintained in an Excel sheet under folder Test Cases and Execution Report)
2. Automated test cases - 4 from the above test cases automated as below:

  a. InvalidSearch: TC - 04: To verify that when user types in speacial characters in the search box, no search results are found
  b. SearchCity: TC - 01: To verify if user is able to search a city using the search box
  c. SearchCityAlternateAlphabets: TC - 05: To verify that when user types in alternate albhabets in the search box, Appropriate search results are displayed
  d. SelectCityfromtheList: TC - 02: To verify if user is able to select a city from the city list

3. Separate Branch created - azmanBranch and a Pull request raised to the master branch
4. Test Execution report (Maintained in an Excel sheet under folder Test Cases and Execution Report)
5. Overall Execution report (Maintained in a PPT under folder Overall Evaluation Report)
</commit_message>
<xml_diff>
--- a/Test Cases and Execution Report/Test Cases and Execution Report.xlsx
+++ b/Test Cases and Execution Report/Test Cases and Execution Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/azansari/Documents/GitHub/mobile-test/Test Cases and Execution Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2635E7-EB2B-6946-96CE-D4E56B8DD8D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAD4D5D-C9A3-D04C-BCE0-52C2F23D41F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F616D8E3-1D36-B54C-A515-2C861EC6B1A8}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="64">
   <si>
     <t>TC - 01: To verify if user is able to search a city using the search box</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>Pre - condition: User has a valid innternet connection</t>
-  </si>
-  <si>
     <t>TC - 02: To verify if user is able to select a city from the city list</t>
   </si>
   <si>
@@ -205,16 +202,28 @@
     <t>Minor</t>
   </si>
   <si>
-    <t>TC - 06: To verify that when user is on the Map screen landing page, Google map is interactable</t>
-  </si>
-  <si>
-    <t>Google Map should be interactable</t>
-  </si>
-  <si>
-    <t>Verify that user is able to interact with the Google Map</t>
-  </si>
-  <si>
-    <t>Google Map is not interactable</t>
+    <t>Pre - condition: Mobile Assignment application is installed in your device</t>
+  </si>
+  <si>
+    <t>TC - 07: To verify that Cities in the list are alphabatically ordered</t>
+  </si>
+  <si>
+    <t>Verify that Cities in the list are alphabatically ordered</t>
+  </si>
+  <si>
+    <t>TC - 08: To verify that when user types a search term in the search box, Cities in the search list are alphabatically ordered</t>
+  </si>
+  <si>
+    <t>Cities displayed in the list should be alphabatically ordered</t>
+  </si>
+  <si>
+    <t>Cities displayed in the list is alphabatically ordered</t>
+  </si>
+  <si>
+    <t>Type alternate albhabets like "A" in the search box</t>
+  </si>
+  <si>
+    <t>The list of the cities staring with 'A' should be displayed</t>
   </si>
 </sst>
 </file>
@@ -471,7 +480,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -493,9 +502,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -522,13 +528,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -540,6 +540,15 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -548,6 +557,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +835,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -2746,38 +2758,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E37929-D6B4-9047-8925-B9A643706CC6}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.6640625" customWidth="1"/>
     <col min="3" max="3" width="65" customWidth="1"/>
     <col min="4" max="4" width="60.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="21">
-      <c r="A2" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
+      <c r="A2" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:5" ht="21">
       <c r="A3" s="1" t="s">
@@ -2866,22 +2878,22 @@
     </row>
     <row r="9" spans="1:5" ht="17" thickBot="1"/>
     <row r="10" spans="1:5" ht="21">
-      <c r="A10" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="1:5" ht="21">
-      <c r="A11" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
+      <c r="A11" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="25"/>
     </row>
     <row r="12" spans="1:5" ht="21">
       <c r="A12" s="1" t="s">
@@ -2908,10 +2920,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>10</v>
@@ -2922,13 +2934,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>10</v>
@@ -2939,7 +2951,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>19</v>
@@ -2970,22 +2982,22 @@
     </row>
     <row r="18" spans="1:5" ht="17" thickBot="1"/>
     <row r="19" spans="1:5" ht="21">
-      <c r="A19" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
+      <c r="A19" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20" spans="1:5" ht="21">
-      <c r="A20" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="22"/>
+      <c r="A20" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="25"/>
     </row>
     <row r="21" spans="1:5" ht="21">
       <c r="A21" s="1" t="s">
@@ -3012,10 +3024,10 @@
         <v>7</v>
       </c>
       <c r="C22" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>10</v>
@@ -3026,13 +3038,13 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>10</v>
@@ -3042,14 +3054,14 @@
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="D24" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>23</v>
@@ -3057,22 +3069,22 @@
     </row>
     <row r="26" spans="1:5" ht="17" thickBot="1"/>
     <row r="27" spans="1:5" ht="21">
-      <c r="A27" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="25"/>
+      <c r="A27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:5" ht="21">
-      <c r="A28" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="22"/>
+      <c r="A28" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:5" ht="21">
       <c r="A29" s="1" t="s">
@@ -3099,10 +3111,10 @@
         <v>7</v>
       </c>
       <c r="C30" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>10</v>
@@ -3113,13 +3125,13 @@
         <v>11</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E31" s="7" t="s">
         <v>10</v>
@@ -3127,22 +3139,22 @@
     </row>
     <row r="33" spans="1:5" ht="17" thickBot="1"/>
     <row r="34" spans="1:5" ht="21">
-      <c r="A34" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
+      <c r="A34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="1:5" ht="21">
-      <c r="A35" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="22"/>
+      <c r="A35" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
     </row>
     <row r="36" spans="1:5" ht="21">
       <c r="A36" s="1" t="s">
@@ -3169,10 +3181,10 @@
         <v>7</v>
       </c>
       <c r="C37" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>10</v>
@@ -3183,13 +3195,13 @@
         <v>11</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E38" s="7" t="s">
         <v>10</v>
@@ -3197,22 +3209,22 @@
     </row>
     <row r="40" spans="1:5" ht="17" thickBot="1"/>
     <row r="41" spans="1:5" ht="21">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42" spans="1:5" ht="21">
-      <c r="A42" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-      <c r="D42" s="21"/>
-      <c r="E42" s="22"/>
+      <c r="A42" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="25"/>
     </row>
     <row r="43" spans="1:5" ht="21">
       <c r="A43" s="1" t="s">
@@ -3235,72 +3247,127 @@
       <c r="A44" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C44" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="19" t="s">
         <v>26</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="21">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:5" ht="45" thickBot="1">
+      <c r="A45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="2" t="s">
+      <c r="B45" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="17" thickBot="1"/>
+    <row r="48" spans="1:5" ht="21">
+      <c r="A48" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="22"/>
+    </row>
+    <row r="49" spans="1:5" ht="21">
+      <c r="A49" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="25"/>
+    </row>
+    <row r="50" spans="1:5" ht="21">
+      <c r="A50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="44">
+      <c r="A51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="21">
+      <c r="A52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="7" t="s">
+      <c r="E52" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="21">
-      <c r="A46" s="4" t="s">
+    <row r="53" spans="1:5" ht="45" thickBot="1">
+      <c r="A53" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="7" t="s">
+      <c r="B53" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="45" thickBot="1">
-      <c r="A47" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="A48:E48"/>
+    <mergeCell ref="A49:E49"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A1:E1"/>
@@ -3323,7 +3390,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9746B214-D07B-1849-8E83-C031B1040D3A}">
   <dimension ref="D5:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -3337,7 +3406,7 @@
     <row r="5" spans="4:9" ht="17" thickBot="1"/>
     <row r="6" spans="4:9" ht="24">
       <c r="D6" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="27"/>
       <c r="F6" s="27"/>
@@ -3346,79 +3415,79 @@
       <c r="I6" s="28"/>
     </row>
     <row r="7" spans="4:9" ht="44">
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="H7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="18" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="4:9" ht="22" thickBot="1">
       <c r="D8" s="8">
-        <v>6</v>
-      </c>
-      <c r="E8" s="15">
-        <v>2</v>
-      </c>
-      <c r="F8" s="15">
+        <v>8</v>
+      </c>
+      <c r="E8" s="14">
         <v>4</v>
       </c>
-      <c r="G8" s="15">
-        <v>19</v>
-      </c>
-      <c r="H8" s="15">
-        <v>15</v>
-      </c>
-      <c r="I8" s="16">
+      <c r="F8" s="14">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14">
+        <v>24</v>
+      </c>
+      <c r="H8" s="14">
+        <v>20</v>
+      </c>
+      <c r="I8" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="5:8" ht="17" thickBot="1"/>
     <row r="24" spans="5:8" ht="24">
       <c r="E24" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F24" s="27"/>
       <c r="G24" s="27"/>
       <c r="H24" s="28"/>
     </row>
     <row r="25" spans="5:8" ht="44">
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="H25" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H25" s="18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="26" spans="5:8" ht="22" thickBot="1">
       <c r="E26" s="8">
         <v>4</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="12">
         <v>3</v>
       </c>
-      <c r="G26" s="13">
+      <c r="G26" s="12">
         <v>1</v>
       </c>
-      <c r="H26" s="14">
+      <c r="H26" s="13">
         <v>0</v>
       </c>
     </row>

</xml_diff>